<commit_message>
Update sur bdd politcis
Erreurs sur la colonne 2002-01
</commit_message>
<xml_diff>
--- a/datasets/DATA_POLITICS.xlsx
+++ b/datasets/DATA_POLITICS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathanpizzetta/Documents/TSE/Cours/M1/Applied econometrics/Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathanpizzetta/Documents/TSE/Cours/M1/Applied econometrics/Code/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC500464-4472-2A4D-9966-82722F0BC47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C518360-5898-9744-9120-9C167453241D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2355" uniqueCount="2337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2350" uniqueCount="2337">
   <si>
     <t>Airport</t>
   </si>
@@ -7385,7 +7385,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ANE6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -10530,8 +10532,8 @@
       <c r="A2" t="s">
         <v>262</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="B2">
+        <v>2293374</v>
       </c>
       <c r="C2" t="s">
         <v>263</v>
@@ -13667,8 +13669,8 @@
       <c r="A3" t="s">
         <v>520</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
+      <c r="B3">
+        <v>1206358</v>
       </c>
       <c r="C3" t="s">
         <v>521</v>
@@ -16804,8 +16806,8 @@
       <c r="A4" t="s">
         <v>778</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
+      <c r="B4">
+        <v>863690</v>
       </c>
       <c r="C4" t="s">
         <v>779</v>
@@ -19941,8 +19943,8 @@
       <c r="A5" t="s">
         <v>1037</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
+      <c r="B5">
+        <v>3318027</v>
       </c>
       <c r="C5" t="s">
         <v>1038</v>
@@ -23078,8 +23080,8 @@
       <c r="A6" t="s">
         <v>1296</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
+      <c r="B6">
+        <v>1587368</v>
       </c>
       <c r="C6" t="s">
         <v>1297</v>

</xml_diff>